<commit_message>
Thuc hanh 5 done
</commit_message>
<xml_diff>
--- a/Buoi5/Data_PhanLopDL.xlsx
+++ b/Buoi5/Data_PhanLopDL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Khai phá dữ liệu\Thực hành\data-mining\Buoi5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2B81AD-7C16-4D15-992A-90B3121A0021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34357441-9B01-48B9-8FB5-12A0CA35B6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25ADC37E-2BD0-4E21-B055-CC33F902A07A}"/>
   </bookViews>
@@ -432,11 +432,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{102C7D17-7A1F-4E1C-8EA1-9BF4BC1DDF52}">
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A475" workbookViewId="0">
-      <selection activeCell="C493" sqref="C493"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>